<commit_message>
added contingency for one row of data
</commit_message>
<xml_diff>
--- a/TablePercents_split.xlsx
+++ b/TablePercents_split.xlsx
@@ -9,19 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="T1" sheetId="2" r:id="rId1"/>
     <sheet name="T2" sheetId="13" r:id="rId2"/>
     <sheet name="T3" sheetId="14" r:id="rId3"/>
+    <sheet name="T4" sheetId="15" r:id="rId4"/>
+    <sheet name="T5" sheetId="16" r:id="rId5"/>
+    <sheet name="T6" sheetId="17" r:id="rId6"/>
+    <sheet name="T7" sheetId="18" r:id="rId7"/>
+    <sheet name="T8" sheetId="19" r:id="rId8"/>
+    <sheet name="T9" sheetId="20" r:id="rId9"/>
+    <sheet name="T10" sheetId="21" r:id="rId10"/>
+    <sheet name="T11" sheetId="22" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="1">
   <si>
     <t>NA</t>
   </si>
@@ -866,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L11"/>
     </sheetView>
   </sheetViews>
@@ -1222,6 +1230,71 @@
       </c>
       <c r="J11">
         <v>0.51120423000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.39470681000000002</v>
+      </c>
+      <c r="B1">
+        <v>0.60529319000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.32634951000000001</v>
+      </c>
+      <c r="B1">
+        <v>0.18079793999999999</v>
+      </c>
+      <c r="C1">
+        <v>0.49285256</v>
       </c>
     </row>
   </sheetData>
@@ -1854,4 +1927,951 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>9.3881870000000006E-2</v>
+      </c>
+      <c r="B1">
+        <v>0.18380008</v>
+      </c>
+      <c r="C1">
+        <v>2.461934E-2</v>
+      </c>
+      <c r="D1">
+        <v>7.2636820000000005E-2</v>
+      </c>
+      <c r="E1">
+        <v>5.90679E-2</v>
+      </c>
+      <c r="F1">
+        <v>3.5903810000000001E-2</v>
+      </c>
+      <c r="G1">
+        <v>3.940946E-2</v>
+      </c>
+      <c r="H1">
+        <v>1.221203E-2</v>
+      </c>
+      <c r="I1">
+        <v>5.6932759999999999E-2</v>
+      </c>
+      <c r="J1">
+        <v>0.14670950999999999</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>3.6636099999999999E-3</v>
+      </c>
+      <c r="M1">
+        <v>0.27116280999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2.840755E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.2771979999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.33300469999999999</v>
+      </c>
+      <c r="F2">
+        <v>2.256122E-2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>5.2458449999999997E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.18095109000000001</v>
+      </c>
+      <c r="J2">
+        <v>5.2204319999999999E-2</v>
+      </c>
+      <c r="K2">
+        <v>2.7172000000000002E-2</v>
+      </c>
+      <c r="L2">
+        <v>1.795043E-2</v>
+      </c>
+      <c r="M2">
+        <v>0.25251825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3.727892E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.1533239999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.7117029999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>3.6737579999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>2.3178130000000002E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.30113136000000001</v>
+      </c>
+      <c r="J3">
+        <v>0.29414318</v>
+      </c>
+      <c r="K3">
+        <v>1.5772520000000002E-2</v>
+      </c>
+      <c r="L3">
+        <v>2.0161889999999998E-2</v>
+      </c>
+      <c r="M3">
+        <v>0.21294615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.22193515</v>
+      </c>
+      <c r="E4">
+        <v>0.17448219000000001</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>6.2222800000000002E-2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>6.5882960000000004E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.27270379</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>5.2706370000000002E-2</v>
+      </c>
+      <c r="M4">
+        <v>0.15006674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.11703692</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5.9447319999999998E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.36400052999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.27482839999999997</v>
+      </c>
+      <c r="K5">
+        <v>3.000947E-2</v>
+      </c>
+      <c r="L5">
+        <v>2.3407379999999998E-2</v>
+      </c>
+      <c r="M5">
+        <v>0.13126998000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.23880675000000001</v>
+      </c>
+      <c r="G6">
+        <v>5.1994449999999998E-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>8.0880259999999995E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.12998613000000001</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.49833241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>3.9155759999999998E-2</v>
+      </c>
+      <c r="G7">
+        <v>5.252602E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.9577879999999999E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.26236635000000003</v>
+      </c>
+      <c r="J7">
+        <v>0.48844199999999999</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>8.6190429999999998E-2</v>
+      </c>
+      <c r="M7">
+        <v>5.1741540000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>3.9155759999999998E-2</v>
+      </c>
+      <c r="G8">
+        <v>5.252602E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.9577879999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.26236635000000003</v>
+      </c>
+      <c r="J8">
+        <v>0.48844199999999999</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>8.6190429999999998E-2</v>
+      </c>
+      <c r="M8">
+        <v>5.1741540000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>4.761485E-2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.69411803000000005</v>
+      </c>
+      <c r="J9">
+        <v>0.19001915999999999</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>6.8247959999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>4.761485E-2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.69411803000000005</v>
+      </c>
+      <c r="J10">
+        <v>0.19001915999999999</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>6.8247959999999996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4.761485E-2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.69411803000000005</v>
+      </c>
+      <c r="J11">
+        <v>0.19001915999999999</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>6.8247959999999996E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4.5008380000000001E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.46071764999999998</v>
+      </c>
+      <c r="J12">
+        <v>0.38180598999999998</v>
+      </c>
+      <c r="K12">
+        <v>6.1082810000000001E-2</v>
+      </c>
+      <c r="L12">
+        <v>5.9221600000000001E-3</v>
+      </c>
+      <c r="M12">
+        <v>4.5463009999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.10683694000000001</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0.89316306000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0.33693182999999999</v>
+      </c>
+      <c r="L14">
+        <v>0.20891526999999999</v>
+      </c>
+      <c r="M14">
+        <v>0.45415290000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2.4330460000000002E-2</v>
+      </c>
+      <c r="B1">
+        <v>1.8365289999999999E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.95730424999999997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.10894186</v>
+      </c>
+      <c r="B2">
+        <v>7.7379509999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.81367862999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9.82962E-2</v>
+      </c>
+      <c r="B3">
+        <v>2.7522939999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.87418087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>5.3825449999999997E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.94617454999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>7.5636629999999996E-2</v>
+      </c>
+      <c r="B1">
+        <v>2.932301E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.11732059</v>
+      </c>
+      <c r="D1">
+        <v>0.77771977999999997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.17099511000000001</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.82900488999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.32228361</v>
+      </c>
+      <c r="D3">
+        <v>0.67771638999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.12020328</v>
+      </c>
+      <c r="B1">
+        <v>4.2835379999999999E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.83696135000000005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.36083258000000001</v>
+      </c>
+      <c r="B2">
+        <v>4.475428E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.59441314000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>6.9467370000000001E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.93053262999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.21006196999999999</v>
+      </c>
+      <c r="B1">
+        <v>6.2031459999999997E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.72790657000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.42584423999999999</v>
+      </c>
+      <c r="B2">
+        <v>8.3527439999999994E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.49062832000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.15427610999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.84572389000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.30519223000000001</v>
+      </c>
+      <c r="B1">
+        <v>0.69480777000000005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed for dealing with 100% and adjusting >0% and <100%
</commit_message>
<xml_diff>
--- a/TablePercents_split.xlsx
+++ b/TablePercents_split.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="T1" sheetId="2" r:id="rId1"/>
@@ -1280,7 +1280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1306,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added checks for row and column names
</commit_message>
<xml_diff>
--- a/TablePercents_split.xlsx
+++ b/TablePercents_split.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="T1" sheetId="2" r:id="rId1"/>
@@ -1362,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1535,7 +1535,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1569,7 @@
         <v>5390</v>
       </c>
       <c r="K1">
-        <v>5396</v>
+        <v>5398</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3105,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,12 +3119,12 @@
         <v>5746</v>
       </c>
       <c r="D1">
-        <v>57554</v>
+        <v>5754</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6702</v>
+        <v>5702</v>
       </c>
       <c r="B2">
         <v>0.12020328</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6814</v>
+        <v>5810</v>
       </c>
       <c r="B3">
         <v>0.36083258000000001</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6838</v>
+        <v>5834</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>

</xml_diff>